<commit_message>
Fixed country code input and updated WebDriver path
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -335,6 +335,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,7 +629,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>